<commit_message>
Removed analysis worksheet that was generated.
</commit_message>
<xml_diff>
--- a/excel/DEMO Copilot in Excel Extravaganza.xlsx
+++ b/excel/DEMO Copilot in Excel Extravaganza.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerd/Development/@copilot/@copilot-prompts/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{184331BA-14FD-BD4B-9BB2-040FA4F77951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2129C884-EE74-8A4D-84BB-04A70E8FB07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="860" windowWidth="25060" windowHeight="20360" firstSheet="1" activeTab="1" xr2:uid="{FCF803C5-C09F-45BC-8C9D-68DAA79B3696}"/>
+    <workbookView xWindow="25780" yWindow="860" windowWidth="25060" windowHeight="20360" firstSheet="2" activeTab="10" xr2:uid="{FCF803C5-C09F-45BC-8C9D-68DAA79B3696}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="Learn" sheetId="18" r:id="rId9"/>
     <sheet name="Advanced Analytics" sheetId="13" r:id="rId10"/>
     <sheet name="Search the Web" sheetId="14" r:id="rId11"/>
-    <sheet name="Analysis1" sheetId="19" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="Revenue_Accelerator">Highlighting!$H$4</definedName>
@@ -51,11 +50,10 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="17">
+  <futureMetadata name="XLRICHVALUE" count="11">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -133,64 +131,8 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="737"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="734"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="741"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="744"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="747"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="751"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </cellMetadata>
-  <valueMetadata count="17">
+  <valueMetadata count="11">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -224,24 +166,6 @@
     <bk>
       <rc t="1" v="10"/>
     </bk>
-    <bk>
-      <rc t="1" v="11"/>
-    </bk>
-    <bk>
-      <rc t="1" v="12"/>
-    </bk>
-    <bk>
-      <rc t="1" v="13"/>
-    </bk>
-    <bk>
-      <rc t="1" v="14"/>
-    </bk>
-    <bk>
-      <rc t="1" v="15"/>
-    </bk>
-    <bk>
-      <rc t="1" v="16"/>
-    </bk>
   </valueMetadata>
 </metadata>
 </file>
@@ -263,65 +187,11 @@
 </code>
     </initialization>
   </environmentDefinition>
-  <pythonScripts>
-    <pythonScript>
-      <code>Table8_df=xl(%P2%, headers=True)</code>
-    </pythonScript>
-    <pythonScript>
-      <code>#Distribution of patient satisfaction scores
-# Analyze satisfaction scores distribution
-plt.rcParams['font.family'] = ['Meiryo','Batang','TH SarabunPSK','SimHei','DejaVu Sans']
-plt.figure(figsize=(10, 6))
-# Plot satisfaction score distribution
-sns.histplot(Table8_df['sat_score'], bins=5, kde=True, color='blue')
-plt.title('Distribution of Patient Satisfaction Scores')
-plt.xlabel('Satisfaction Score')
-plt.ylabel('Frequency')
-plt.grid(axis='y', linestyle='--', alpha=0.7)
-plt.show()</code>
-    </pythonScript>
-    <pythonScript>
-      <code>#Sentiment analysis on patient comments
-# Sentiment analysis on patient comments
-from nltk.sentiment.vader import SentimentIntensityAnalyzer
-import nltk
-nltk.download('vader_lexicon')
-# Initialize sentiment analyzer
-sid = SentimentIntensityAnalyzer()
-# Perform sentiment analysis on comments
-Table8_df['sentiment_score'] = Table8_df['comments'].fillna('').apply(lambda x: sid.polarity_scores(x)['compound'])
-# Display sentiment scores
-Table8_df[['comments', 'sentiment_score']].head()</code>
-    </pythonScript>
-    <pythonScript>
-      <code>#Correlation between satisfaction scores and sentiment scores
-#Correlation between satisfaction scores and sentiment scores
-# Calculate correlation between satisfaction scores and sentiment scores
-correlation = Table8_df[['sat_score', 'sentiment_score']].corr()
-# Display correlation matrix
-correlation</code>
-    </pythonScript>
-    <pythonScript>
-      <code>#Scatter plot of satisfaction scores vs sentiment scores
-#Visualize the relationship between satisfaction scores and sentiment scores
-# Scatter plot to visualize the relationship
-plt.rcParams['font.family'] = ['Meiryo','Batang','TH SarabunPSK','SimHei','DejaVu Sans']
-plt.figure(figsize=(10, 6))
-# Scatter plot
-sns.scatterplot(data=Table8_df, x='sat_score', y='sentiment_score', hue='sat_score', palette='viridis', alpha=0.7)
-plt.title('Relationship Between Satisfaction Scores and Sentiment Scores')
-plt.xlabel('Satisfaction Score')
-plt.ylabel('Sentiment Score')
-plt.grid(axis='y', linestyle='--', alpha=0.7)
-plt.legend(title='Satisfaction Score', loc='upper left')
-plt.show()</code>
-    </pythonScript>
-  </pythonScripts>
 </python>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="1775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2531" uniqueCount="1767">
   <si>
     <t>Explore tips and tricks for working with dates.</t>
   </si>
@@ -5622,30 +5492,6 @@
   </si>
   <si>
     <t>Create a table from web search of top 15 companies in the S&amp;P 500 and their market cap</t>
-  </si>
-  <si>
-    <t>Analysis Sheet</t>
-  </si>
-  <si>
-    <t>This sheet will include all the Python formulas generated by Copilot.</t>
-  </si>
-  <si>
-    <t>Load data from Advanced Analytics, Table8</t>
-  </si>
-  <si>
-    <t>Preview</t>
-  </si>
-  <si>
-    <t>Distribution of patient satisfaction scores</t>
-  </si>
-  <si>
-    <t>Sentiment analysis on patient comments</t>
-  </si>
-  <si>
-    <t>Correlation between satisfaction scores and sentiment scores</t>
-  </si>
-  <si>
-    <t>Scatter plot of satisfaction scores vs sentiment scores</t>
   </si>
 </sst>
 </file>
@@ -5657,7 +5503,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5712,30 +5558,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color rgb="FF156082"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF156082"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5811,7 +5633,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5883,9 +5705,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6327,119 +6146,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419030</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" title="Distribution of patient satisfaction scores">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D69D3E62-4D58-BF91-CEBC-A374E219BEFE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-          <a:extLst>
-            <a:ext uri="{53484399-7A02-498B-ADA4-41CD10E50FAC}">
-              <aif:imageFormula xmlns:aif="http://schemas.microsoft.com/office/drawing/2022/imageformula" formula="Analysis1!A24"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="4886325"/>
-          <a:ext cx="4686230" cy="3048000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>558336</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" title="Scatter plot of satisfaction scores vs sentiment scores">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E5494D5-1188-EC33-F202-582966DBBB24}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-          <a:extLst>
-            <a:ext uri="{53484399-7A02-498B-ADA4-41CD10E50FAC}">
-              <aif:imageFormula xmlns:aif="http://schemas.microsoft.com/office/drawing/2022/imageformula" formula="Analysis1!A65"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="12858750"/>
-          <a:ext cx="4825536" cy="3048000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -6649,7 +6355,7 @@
 </file>
 
 <file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="41">
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="36">
   <a r="4">
     <v t="r">21</v>
     <v t="r">22</v>
@@ -7014,196 +6720,11 @@
     <v t="s">Greenwich Mean Time</v>
     <v t="s">Western European Time</v>
   </a>
-  <a r="12" c="12">
-    <v t="s"/>
-    <v t="s">id</v>
-    <v t="s">first_name</v>
-    <v t="s">last_name</v>
-    <v t="s">icd10</v>
-    <v t="s">gender</v>
-    <v t="s">...</v>
-    <v t="s">length_of_stay</v>
-    <v t="s">email_address</v>
-    <v t="s">locatiion</v>
-    <v t="s">sat_score</v>
-    <v t="s">comments</v>
-    <v>0</v>
-    <v>1</v>
-    <v t="s">Anjanette</v>
-    <v t="s">Havard</v>
-    <v t="s">H44821</v>
-    <v t="s">Agender</v>
-    <v t="s">...</v>
-    <v>6</v>
-    <v t="s">ahavard0@utexas.edu</v>
-    <v t="s">Northwest Pineview</v>
-    <v>5</v>
-    <v t="s">wonderful stay! Very happy and feeling healthy again.</v>
-    <v>1</v>
-    <v>2</v>
-    <v t="s">Lorrayne</v>
-    <v t="s">Diggens</v>
-    <v t="s">S23152D</v>
-    <v t="s">Female</v>
-    <v t="s">...</v>
-    <v>3</v>
-    <v t="s">ldiggens1@gmpg.org</v>
-    <v t="s">Northwest Pineview</v>
-    <v>5</v>
-    <v t="r">734</v>
-    <v>2</v>
-    <v>3</v>
-    <v t="s">Donny</v>
-    <v t="s">Hindhaugh</v>
-    <v t="s">S8292</v>
-    <v t="s">Male</v>
-    <v t="s">...</v>
-    <v>3</v>
-    <v t="s">dhindhaugh2@ocn.ne.jp</v>
-    <v t="s">Northwest Pineview</v>
-    <v>4</v>
-    <v t="r">734</v>
-    <v>3</v>
-    <v>4</v>
-    <v t="s">Alameda</v>
-    <v t="s">Goldsack</v>
-    <v t="s">S62145P</v>
-    <v t="s">Female</v>
-    <v t="s">...</v>
-    <v>4</v>
-    <v t="s">agoldsack3@mysql.com</v>
-    <v t="s">Northwest Pineview</v>
-    <v>4</v>
-    <v t="r">734</v>
-    <v>4</v>
-    <v>5</v>
-    <v t="s">Gretchen</v>
-    <v t="s">Sobey</v>
-    <v t="s">S43303S</v>
-    <v t="s">Female</v>
-    <v t="s">...</v>
-    <v>3</v>
-    <v t="s">gsobey4@vimeo.com</v>
-    <v t="s">Northwest Pineview</v>
-    <v>5</v>
-    <v t="r">734</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v t="s">...</v>
-    <v>265</v>
-    <v>266</v>
-    <v t="s">Shay</v>
-    <v t="s">Gabbotts</v>
-    <v t="s">S42034S</v>
-    <v t="s">Female</v>
-    <v t="s">...</v>
-    <v>2</v>
-    <v t="s">sgabbotts7d@fc2.com</v>
-    <v t="s">Glenview Central</v>
-    <v>2</v>
-    <v t="r">734</v>
-    <v>266</v>
-    <v>267</v>
-    <v t="s">Eamon</v>
-    <v t="s">Fetteplace</v>
-    <v t="s">K007</v>
-    <v t="s">Male</v>
-    <v t="s">...</v>
-    <v>4</v>
-    <v t="s">efetteplace7e@nps.gov</v>
-    <v t="s">Glenview Central</v>
-    <v>4</v>
-    <v t="r">734</v>
-    <v>267</v>
-    <v>268</v>
-    <v t="s">Darda</v>
-    <v t="s">Shewry</v>
-    <v t="s">S86001</v>
-    <v t="s">Genderfluid</v>
-    <v t="s">...</v>
-    <v>1</v>
-    <v t="s">dshewry7f@senate.gov</v>
-    <v t="s">Glenview Central</v>
-    <v>5</v>
-    <v t="r">734</v>
-    <v>268</v>
-    <v>269</v>
-    <v t="s">Arne</v>
-    <v t="s">Robbe</v>
-    <v t="s">H02106</v>
-    <v t="s">Male</v>
-    <v t="s">...</v>
-    <v>2</v>
-    <v t="s">arobbe7g@ning.com</v>
-    <v t="s">Glenview Central</v>
-    <v>5</v>
-    <v t="r">734</v>
-    <v>269</v>
-    <v>270</v>
-    <v t="s">Biron</v>
-    <v t="s">Quodling</v>
-    <v t="s">S52009K</v>
-    <v t="s">Male</v>
-    <v t="s">...</v>
-    <v>2</v>
-    <v t="s">bquodling7h@google.com</v>
-    <v t="s">Glenview Central</v>
-    <v>2</v>
-    <v t="r">734</v>
-  </a>
-  <a r="2">
-    <v>841</v>
-    <v>547</v>
-  </a>
-  <a r="6" c="3">
-    <v t="s"/>
-    <v t="s">comments</v>
-    <v t="s">sentiment_score</v>
-    <v>0</v>
-    <v t="s">wonderful stay! Very happy and feeling healthy again.</v>
-    <v>0.90900000000000003</v>
-    <v>1</v>
-    <v t="r">734</v>
-    <v>0</v>
-    <v>2</v>
-    <v t="r">734</v>
-    <v>0</v>
-    <v>3</v>
-    <v t="r">734</v>
-    <v>0</v>
-    <v>4</v>
-    <v t="r">734</v>
-    <v>0</v>
-  </a>
-  <a r="3" c="3">
-    <v t="s"/>
-    <v t="s">sat_score</v>
-    <v t="s">sentiment_score</v>
-    <v t="s">sat_score</v>
-    <v>1</v>
-    <v>0.44649993297971607</v>
-    <v t="s">sentiment_score</v>
-    <v>0.44649993297971607</v>
-    <v>1</v>
-  </a>
-  <a r="2">
-    <v>866</v>
-    <v>547</v>
-  </a>
 </arrayData>
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="752">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="734">
   <rv s="0">
     <v>536870912</v>
     <v>United States</v>
@@ -11687,108 +11208,11 @@
     <v>732</v>
     <v>mdp/vdpid/242</v>
   </rv>
-  <rv s="1">
-    <fb>0</fb>
-    <v>97</v>
-  </rv>
-  <rv s="3">
-    <v>36</v>
-  </rv>
-  <rv s="9">
-    <v>DataFrame</v>
-    <v>96</v>
-    <v>735</v>
-  </rv>
-  <rv s="10">
-    <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
-    <v>DataFrame</v>
-    <v xml:space="preserve">      id first_name   last_name    icd10       gender       date  \
-0      1  Anjanette      Havard   H44821      Agender 2024-09-06   
-1      2   Lorrayne     Diggens  S23152D       Female 2024-08-27   
-2      3      Donny   Hindhaugh    S8292        ...</v>
-    <v>736</v>
-    <v>98</v>
-  </rv>
-  <rv s="11">
-    <v>0</v>
-    <v>9</v>
-  </rv>
-  <rv s="3">
-    <v>37</v>
-  </rv>
-  <rv s="12">
-    <v>Image</v>
-    <v>99</v>
-    <v>738</v>
-    <v>739</v>
-  </rv>
-  <rv s="10">
-    <v>&lt;class 'PIL.PngImagePlugin.PngImageFile'&gt;</v>
-    <v>PngImageFile</v>
-    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=841x547 at 0x7F9134EB4950&gt;</v>
-    <v>740</v>
-    <v>98</v>
-  </rv>
-  <rv s="3">
-    <v>38</v>
-  </rv>
-  <rv s="9">
-    <v>DataFrame</v>
-    <v>101</v>
-    <v>742</v>
-  </rv>
-  <rv s="10">
-    <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
-    <v>DataFrame</v>
-    <v xml:space="preserve">                                            comments  sentiment_score
-0  wonderful stay! Very happy and feeling healthy...            0.909
-1                                               None            0.000
-2                                         ...</v>
-    <v>743</v>
-    <v>98</v>
-  </rv>
-  <rv s="3">
-    <v>39</v>
-  </rv>
-  <rv s="9">
-    <v>DataFrame</v>
-    <v>103</v>
-    <v>745</v>
-  </rv>
-  <rv s="10">
-    <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
-    <v>DataFrame</v>
-    <v xml:space="preserve">                 sat_score  sentiment_score
-sat_score           1.0000           0.4465
-sentiment_score     0.4465           1.0000</v>
-    <v>746</v>
-    <v>98</v>
-  </rv>
-  <rv s="11">
-    <v>1</v>
-    <v>9</v>
-  </rv>
-  <rv s="3">
-    <v>40</v>
-  </rv>
-  <rv s="12">
-    <v>Image</v>
-    <v>99</v>
-    <v>748</v>
-    <v>749</v>
-  </rv>
-  <rv s="10">
-    <v>&lt;class 'PIL.PngImagePlugin.PngImageFile'&gt;</v>
-    <v>PngImageFile</v>
-    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=866x547 at 0x7F9123736630&gt;</v>
-    <v>750</v>
-    <v>98</v>
-  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="13">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
   <s t="_linkedentity2">
     <k n="%EntityServiceId" t="i"/>
     <k n="_DisplayString" t="s"/>
@@ -12070,28 +11494,6 @@
     <k n="Urban population" t="r"/>
     <k n="VDPID/VSID" t="s"/>
   </s>
-  <s t="_entity">
-    <k n="_DisplayString" t="s"/>
-    <k n="_ViewInfo" t="spb"/>
-    <k n="arrayPreview" t="r"/>
-  </s>
-  <s t="_python">
-    <k n="Python_type" t="s"/>
-    <k n="Python_typeName" t="s"/>
-    <k n="Python_str" t="s"/>
-    <k n="preview" t="r"/>
-    <k n="_Provider" t="spb"/>
-  </s>
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-  <s t="_entity">
-    <k n="_DisplayString" t="s"/>
-    <k n="_Format" t="spb"/>
-    <k n="image" t="r"/>
-    <k n="size" t="r"/>
-  </s>
 </rvStructures>
 </file>
 
@@ -12351,7 +11753,7 @@
       <v t="s">Description</v>
     </a>
   </spbArrays>
-  <spbData count="104">
+  <spbData count="95">
     <spb s="0">
       <v xml:space="preserve">data.worldbank.org	</v>
       <v xml:space="preserve">	</v>
@@ -13648,53 +13050,12 @@
       <v>2017</v>
       <v>2019</v>
     </spb>
-    <spb s="13">
-      <v>270</v>
-      <v>11</v>
-      <v>DataFrame</v>
-      <v>arrayPreview</v>
-      <v>1</v>
-    </spb>
-    <spb s="14">
-      <v>95</v>
-    </spb>
-    <spb s="8">
-      <v>12</v>
-    </spb>
-    <spb s="6">
-      <v>https://www.anaconda.com/excel</v>
-      <v>https://res.cdn.office.net/officepysvc/prod-msit/anacondalogo.png</v>
-      <v>Python provided by Anaconda</v>
-    </spb>
-    <spb s="15">
-      <v>2</v>
-    </spb>
-    <spb s="13">
-      <v>5</v>
-      <v>2</v>
-      <v>DataFrame</v>
-      <v>arrayPreview</v>
-      <v>1</v>
-    </spb>
-    <spb s="14">
-      <v>100</v>
-    </spb>
-    <spb s="13">
-      <v>2</v>
-      <v>2</v>
-      <v>DataFrame</v>
-      <v>arrayPreview</v>
-      <v>1</v>
-    </spb>
-    <spb s="14">
-      <v>102</v>
-    </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="16">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="13">
   <s>
     <k n="SourceText" t="s"/>
     <k n="LicenseText" t="s"/>
@@ -13969,19 +13330,6 @@
     <k n="Gross tertiary education enrollment (%)" t="spb"/>
     <k n="Population: Labor force participation (%)" t="spb"/>
   </s>
-  <s>
-    <k n="drw" t="i"/>
-    <k n="dcol" t="i"/>
-    <k n="name" t="s"/>
-    <k n="array" t="s"/>
-    <k n="headers" t="b"/>
-  </s>
-  <s>
-    <k n="ArrayCardInfo" t="spb"/>
-  </s>
-  <s>
-    <k n="image" t="i"/>
-  </s>
 </spbStructures>
 </file>
 
@@ -14044,18 +13392,8 @@
       <rpv i="2">_([$$-en-US]* #,##0_);_([$$-en-US]* (#,##0);_([$$-en-US]* "-"_);_(@_)</rpv>
     </rSty>
     <rSty dxfid="0"/>
-    <rSty dxfid="5">
-      <rpv i="2">0;-0;"None"</rpv>
-    </rSty>
   </richStyles>
 </richStyleSheet>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-</richValueRels>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14523,7 +13861,7 @@
       </c>
     </row>
     <row r="3" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
@@ -14531,13 +13869,13 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="32"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="32"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="27" t="s">
         <v>5</v>
       </c>
@@ -14575,10 +13913,10 @@
       </c>
     </row>
     <row r="12" spans="2:3" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -14621,13 +13959,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
@@ -14636,78 +13974,78 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>644</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="38.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>645</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="32" t="s">
         <v>646</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>647</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="32" t="s">
         <v>648</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="32" t="s">
         <v>649</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="32" t="s">
         <v>650</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="22" t="s">
@@ -23745,7 +23083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EBEFE7-4AD6-734F-9796-71DEE02CAD5F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
@@ -23755,13 +23093,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
@@ -23770,41 +23108,41 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>1765</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>1766</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -23821,665 +23159,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD1275D-5F42-461A-9040-C522895EDAA0}">
-  <dimension ref="A1:L65"/>
-  <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="e" cm="1" vm="12">
-        <f t="array" ref="A6">_xlfn._xlws.PY(0,1,Table8[[#Headers],[#Data]])</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="str" cm="1">
-        <f t="array" ref="A9:L20">IFERROR(_FV(A6,"arrayPreview"),_xlfn._DF_Python_str(A6))</f>
-        <v/>
-      </c>
-      <c r="B9" t="str">
-        <v>id</v>
-      </c>
-      <c r="C9" t="str">
-        <v>first_name</v>
-      </c>
-      <c r="D9" t="str">
-        <v>last_name</v>
-      </c>
-      <c r="E9" t="str">
-        <v>icd10</v>
-      </c>
-      <c r="F9" t="str">
-        <v>gender</v>
-      </c>
-      <c r="G9" t="str">
-        <v>...</v>
-      </c>
-      <c r="H9" t="str">
-        <v>length_of_stay</v>
-      </c>
-      <c r="I9" t="str">
-        <v>email_address</v>
-      </c>
-      <c r="J9" t="str">
-        <v>locatiion</v>
-      </c>
-      <c r="K9" t="str">
-        <v>sat_score</v>
-      </c>
-      <c r="L9" t="str">
-        <v>comments</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Anjanette</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Havard</v>
-      </c>
-      <c r="E10" t="str">
-        <v>H44821</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Agender</v>
-      </c>
-      <c r="G10" t="str">
-        <v>...</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10" t="str">
-        <v>ahavard0@utexas.edu</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Northwest Pineview</v>
-      </c>
-      <c r="K10">
-        <v>5</v>
-      </c>
-      <c r="L10" t="str">
-        <v>wonderful stay! Very happy and feeling healthy again.</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Lorrayne</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Diggens</v>
-      </c>
-      <c r="E11" t="str">
-        <v>S23152D</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Female</v>
-      </c>
-      <c r="G11" t="str">
-        <v>...</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11" t="str">
-        <v>ldiggens1@gmpg.org</v>
-      </c>
-      <c r="J11" t="str">
-        <v>Northwest Pineview</v>
-      </c>
-      <c r="K11">
-        <v>5</v>
-      </c>
-      <c r="L11" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Donny</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Hindhaugh</v>
-      </c>
-      <c r="E12" t="str">
-        <v>S8292</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Male</v>
-      </c>
-      <c r="G12" t="str">
-        <v>...</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12" t="str">
-        <v>dhindhaugh2@ocn.ne.jp</v>
-      </c>
-      <c r="J12" t="str">
-        <v>Northwest Pineview</v>
-      </c>
-      <c r="K12">
-        <v>4</v>
-      </c>
-      <c r="L12" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Alameda</v>
-      </c>
-      <c r="D13" t="str">
-        <v>Goldsack</v>
-      </c>
-      <c r="E13" t="str">
-        <v>S62145P</v>
-      </c>
-      <c r="F13" t="str">
-        <v>Female</v>
-      </c>
-      <c r="G13" t="str">
-        <v>...</v>
-      </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-      <c r="I13" t="str">
-        <v>agoldsack3@mysql.com</v>
-      </c>
-      <c r="J13" t="str">
-        <v>Northwest Pineview</v>
-      </c>
-      <c r="K13">
-        <v>4</v>
-      </c>
-      <c r="L13" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Gretchen</v>
-      </c>
-      <c r="D14" t="str">
-        <v>Sobey</v>
-      </c>
-      <c r="E14" t="str">
-        <v>S43303S</v>
-      </c>
-      <c r="F14" t="str">
-        <v>Female</v>
-      </c>
-      <c r="G14" t="str">
-        <v>...</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14" t="str">
-        <v>gsobey4@vimeo.com</v>
-      </c>
-      <c r="J14" t="str">
-        <v>Northwest Pineview</v>
-      </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="L14" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
-        <v>...</v>
-      </c>
-      <c r="B15" t="str">
-        <v>...</v>
-      </c>
-      <c r="C15" t="str">
-        <v>...</v>
-      </c>
-      <c r="D15" t="str">
-        <v>...</v>
-      </c>
-      <c r="E15" t="str">
-        <v>...</v>
-      </c>
-      <c r="F15" t="str">
-        <v>...</v>
-      </c>
-      <c r="G15" t="str">
-        <v>...</v>
-      </c>
-      <c r="H15" t="str">
-        <v>...</v>
-      </c>
-      <c r="I15" t="str">
-        <v>...</v>
-      </c>
-      <c r="J15" t="str">
-        <v>...</v>
-      </c>
-      <c r="K15" t="str">
-        <v>...</v>
-      </c>
-      <c r="L15" t="str">
-        <v>...</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>265</v>
-      </c>
-      <c r="B16">
-        <v>266</v>
-      </c>
-      <c r="C16" t="str">
-        <v>Shay</v>
-      </c>
-      <c r="D16" t="str">
-        <v>Gabbotts</v>
-      </c>
-      <c r="E16" t="str">
-        <v>S42034S</v>
-      </c>
-      <c r="F16" t="str">
-        <v>Female</v>
-      </c>
-      <c r="G16" t="str">
-        <v>...</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16" t="str">
-        <v>sgabbotts7d@fc2.com</v>
-      </c>
-      <c r="J16" t="str">
-        <v>Glenview Central</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>266</v>
-      </c>
-      <c r="B17">
-        <v>267</v>
-      </c>
-      <c r="C17" t="str">
-        <v>Eamon</v>
-      </c>
-      <c r="D17" t="str">
-        <v>Fetteplace</v>
-      </c>
-      <c r="E17" t="str">
-        <v>K007</v>
-      </c>
-      <c r="F17" t="str">
-        <v>Male</v>
-      </c>
-      <c r="G17" t="str">
-        <v>...</v>
-      </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-      <c r="I17" t="str">
-        <v>efetteplace7e@nps.gov</v>
-      </c>
-      <c r="J17" t="str">
-        <v>Glenview Central</v>
-      </c>
-      <c r="K17">
-        <v>4</v>
-      </c>
-      <c r="L17" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>267</v>
-      </c>
-      <c r="B18">
-        <v>268</v>
-      </c>
-      <c r="C18" t="str">
-        <v>Darda</v>
-      </c>
-      <c r="D18" t="str">
-        <v>Shewry</v>
-      </c>
-      <c r="E18" t="str">
-        <v>S86001</v>
-      </c>
-      <c r="F18" t="str">
-        <v>Genderfluid</v>
-      </c>
-      <c r="G18" t="str">
-        <v>...</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18" t="str">
-        <v>dshewry7f@senate.gov</v>
-      </c>
-      <c r="J18" t="str">
-        <v>Glenview Central</v>
-      </c>
-      <c r="K18">
-        <v>5</v>
-      </c>
-      <c r="L18" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>268</v>
-      </c>
-      <c r="B19">
-        <v>269</v>
-      </c>
-      <c r="C19" t="str">
-        <v>Arne</v>
-      </c>
-      <c r="D19" t="str">
-        <v>Robbe</v>
-      </c>
-      <c r="E19" t="str">
-        <v>H02106</v>
-      </c>
-      <c r="F19" t="str">
-        <v>Male</v>
-      </c>
-      <c r="G19" t="str">
-        <v>...</v>
-      </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-      <c r="I19" t="str">
-        <v>arobbe7g@ning.com</v>
-      </c>
-      <c r="J19" t="str">
-        <v>Glenview Central</v>
-      </c>
-      <c r="K19">
-        <v>5</v>
-      </c>
-      <c r="L19" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>269</v>
-      </c>
-      <c r="B20">
-        <v>270</v>
-      </c>
-      <c r="C20" t="str">
-        <v>Biron</v>
-      </c>
-      <c r="D20" t="str">
-        <v>Quodling</v>
-      </c>
-      <c r="E20" t="str">
-        <v>S52009K</v>
-      </c>
-      <c r="F20" t="str">
-        <v>Male</v>
-      </c>
-      <c r="G20" t="str">
-        <v>...</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20" t="str">
-        <v>bquodling7h@google.com</v>
-      </c>
-      <c r="J20" t="str">
-        <v>Glenview Central</v>
-      </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20" vm="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="e" cm="1" vm="14">
-        <f t="array" ref="A24">_xlfn._xlws.PY(1,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="e" cm="1" vm="15">
-        <f t="array" ref="A44">_xlfn._xlws.PY(2,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="str" cm="1">
-        <f t="array" ref="A47:C52">IFERROR(_FV(A44,"arrayPreview"),_xlfn._DF_Python_str(A44))</f>
-        <v/>
-      </c>
-      <c r="B47" t="str">
-        <v>comments</v>
-      </c>
-      <c r="C47" t="str">
-        <v>sentiment_score</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>0</v>
-      </c>
-      <c r="B48" t="str">
-        <v>wonderful stay! Very happy and feeling healthy again.</v>
-      </c>
-      <c r="C48">
-        <v>0.90900000000000003</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" vm="13">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>2</v>
-      </c>
-      <c r="B50" vm="13">
-        <v>0</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>3</v>
-      </c>
-      <c r="B51" vm="13">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>4</v>
-      </c>
-      <c r="B52" vm="13">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="30" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="e" cm="1" vm="16">
-        <f t="array" ref="A56">_xlfn._xlws.PY(3,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="31" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="str" cm="1">
-        <f t="array" ref="A59:C61">IFERROR(_FV(A56,"arrayPreview"),_xlfn._DF_Python_str(A56))</f>
-        <v/>
-      </c>
-      <c r="B59" t="str">
-        <v>sat_score</v>
-      </c>
-      <c r="C59" t="str">
-        <v>sentiment_score</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="str">
-        <v>sat_score</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>0.44649993297971607</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="str">
-        <v>sentiment_score</v>
-      </c>
-      <c r="B61">
-        <v>0.44649993297971607</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A64" s="30" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="e" cm="1" vm="17">
-        <f t="array" ref="A65">_xlfn._xlws.PY(4,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A9F789-E6D9-472B-B032-3B1372602E04}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -24490,10 +23174,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="D1" s="25" t="s">
         <v>16</v>
       </c>
@@ -24933,13 +23617,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
@@ -24948,23 +23632,23 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -26109,13 +24793,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
@@ -26124,23 +24808,23 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -27891,10 +26575,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="D1" s="25" t="s">
         <v>16</v>
       </c>
@@ -28076,15 +26760,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="I1" s="25" t="s">
         <v>16</v>
       </c>
@@ -28093,14 +26777,14 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>565</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
@@ -29390,13 +28074,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
@@ -29405,34 +28089,34 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>596</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>597</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="32" t="s">
         <v>598</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="G4" t="s">
         <v>599</v>
       </c>
@@ -29444,23 +28128,23 @@
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>600</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="32" t="s">
         <v>601</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
@@ -29552,7 +28236,7 @@
       </c>
       <c r="M10" s="8" t="str">
         <f ca="1">IF(RAND() &lt; 0.5, "Yes", "No")</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="N10" s="8" t="str">
         <f t="shared" ref="N10:O21" ca="1" si="0">IF(RAND() &lt; 0.5, "Yes", "No")</f>
@@ -29606,7 +28290,7 @@
       </c>
       <c r="N11" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O11" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -29652,11 +28336,11 @@
       </c>
       <c r="M12" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="N12" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="O12" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -29702,7 +28386,7 @@
       </c>
       <c r="M13" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="N13" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -29710,7 +28394,7 @@
       </c>
       <c r="O13" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -29750,11 +28434,11 @@
       </c>
       <c r="M14" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="N14" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O14" s="8"/>
     </row>
@@ -29851,7 +28535,7 @@
       </c>
       <c r="N16" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="O16" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -29899,7 +28583,7 @@
       </c>
       <c r="N17" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O17" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -29949,11 +28633,11 @@
       </c>
       <c r="N18" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O18" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="16" x14ac:dyDescent="0.2">
@@ -29999,11 +28683,11 @@
       </c>
       <c r="N19" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="O19" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="16" x14ac:dyDescent="0.2">
@@ -30046,11 +28730,11 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="O20" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="16" x14ac:dyDescent="0.2">
@@ -30136,10 +28820,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="D1" s="25" t="s">
         <v>16</v>
       </c>
@@ -30190,10 +28874,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
@@ -30205,45 +28889,45 @@
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="35" t="s">
         <v>640</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>641</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:7" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="32" t="s">
         <v>642</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>643</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>